<commit_message>
#24 Player prefs set up in the shop scene
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheet.xlsx
+++ b/Documentation/TimeSheet.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eprov\Documents\GitHub\TalosOrigins\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericphilippona/Documents/workspace/TalosOrigins/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="12440"/>
   </bookViews>
   <sheets>
     <sheet name="Team Meetings" sheetId="4" r:id="rId1"/>
@@ -17,9 +17,12 @@
     <sheet name="Philippona" sheetId="2" r:id="rId3"/>
     <sheet name="Ningge" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>DATE</t>
   </si>
@@ -123,12 +126,30 @@
   </si>
   <si>
     <t>UNDOCUMENTED</t>
+  </si>
+  <si>
+    <t>27/10/15</t>
+  </si>
+  <si>
+    <t>28/10/15</t>
+  </si>
+  <si>
+    <t>Breadcrumbs</t>
+  </si>
+  <si>
+    <t>Create Shop UI (includes drag + drop mechanic, particles, upgade cards,…)</t>
+  </si>
+  <si>
+    <t>Grapple research and development + aiming reticle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tweaks to shop UI + Persistence research </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yy/mm/dd;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -170,13 +191,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,22 +489,22 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -486,7 +515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>42262</v>
       </c>
@@ -497,7 +526,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>42265</v>
       </c>
@@ -508,7 +537,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>42267</v>
       </c>
@@ -519,7 +548,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>42269</v>
       </c>
@@ -530,7 +559,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>42276</v>
       </c>
@@ -541,7 +570,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>42291</v>
       </c>
@@ -552,7 +581,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>42292</v>
       </c>
@@ -563,7 +592,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>42295</v>
       </c>
@@ -574,7 +603,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>42297</v>
       </c>
@@ -585,7 +614,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>42300</v>
       </c>
@@ -596,7 +625,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>42301</v>
       </c>
@@ -607,7 +636,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>42304</v>
       </c>
@@ -618,7 +647,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>42306</v>
       </c>
@@ -629,7 +658,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>42308</v>
       </c>
@@ -640,23 +669,23 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
     </row>
@@ -674,14 +703,14 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -692,7 +721,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>42291</v>
       </c>
@@ -703,7 +732,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>42292</v>
       </c>
@@ -714,7 +743,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>42294</v>
       </c>
@@ -725,7 +754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>42295</v>
       </c>
@@ -736,7 +765,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>42297</v>
       </c>
@@ -747,7 +776,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>42299</v>
       </c>
@@ -758,7 +787,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>42300</v>
       </c>
@@ -769,7 +798,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>42301</v>
       </c>
@@ -780,7 +809,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>42304</v>
       </c>
@@ -791,7 +820,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>42307</v>
       </c>
@@ -802,7 +831,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>42308</v>
       </c>
@@ -813,7 +842,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>42308</v>
       </c>
@@ -824,7 +853,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>42309</v>
       </c>
@@ -835,99 +864,99 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="4"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="4"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="4"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="4"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="4"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="4"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="4"/>
     </row>
@@ -942,177 +971,280 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="7"/>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="6">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6"/>
       <c r="D2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="9">
+        <v>42015</v>
+      </c>
+      <c r="B4" s="6">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="9">
+        <v>42015</v>
+      </c>
+      <c r="B5" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
-      <c r="B20" s="4"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
-      <c r="B22" s="4"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
-      <c r="B24" s="4"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
-      <c r="B25" s="4"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
-      <c r="B26" s="4"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
-      <c r="B27" s="4"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
-      <c r="B28" s="4"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
-      <c r="B30" s="4"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
-      <c r="B31" s="4"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
-      <c r="B32" s="4"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
-      <c r="B33" s="4"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
-      <c r="B34" s="4"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
-      <c r="B35" s="4"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
-      <c r="B36" s="4"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
-      <c r="B37" s="4"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
-      <c r="B38" s="4"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
     </row>
   </sheetData>
+  <mergeCells count="38">
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1125,14 +1257,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1143,182 +1275,182 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="4"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="4"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="4"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="4"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="4"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="4"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="4"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Walker Framework for player (not functional yet) + Timesheet
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheet.xlsx
+++ b/Documentation/TimeSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="24240" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="24240" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Team Meetings" sheetId="4" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
   <si>
     <t>DATE</t>
   </si>
@@ -168,6 +168,15 @@
   </si>
   <si>
     <t>Enemy AI groundwork</t>
+  </si>
+  <si>
+    <t>Ressearch into raycast assisted movement stabalization</t>
+  </si>
+  <si>
+    <t>Implementation of racast assisted movement stablization</t>
+  </si>
+  <si>
+    <t>Discussion of tasks splitting for weekend work</t>
   </si>
 </sst>
 </file>
@@ -540,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,23 +730,37 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>42318</v>
+      </c>
+      <c r="B17" s="5">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>42321</v>
+      </c>
+      <c r="B18" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
     </row>
@@ -751,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,12 +995,26 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4"/>
+      <c r="A20" s="3">
+        <v>42322</v>
+      </c>
+      <c r="B20" s="4">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
+      <c r="A21" s="3">
+        <v>42323</v>
+      </c>
+      <c r="B21" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
@@ -1293,30 +1330,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B1:C1"/>
@@ -1331,6 +1344,30 @@
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Audio + New Assets + Fixes + Portal
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheet.xlsx
+++ b/Documentation/TimeSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="24240" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="470" windowWidth="24240" windowHeight="12440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team Meetings" sheetId="4" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
   <si>
     <t>DATE</t>
   </si>
@@ -177,12 +177,15 @@
   </si>
   <si>
     <t>Discussion of tasks splitting for weekend work</t>
+  </si>
+  <si>
+    <t>Missing Audio added + effects and visuals + portal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yy/mm/dd;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -549,23 +552,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C19" sqref="A19:C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -576,7 +579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>42262</v>
       </c>
@@ -587,7 +590,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>42265</v>
       </c>
@@ -598,7 +601,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>42267</v>
       </c>
@@ -609,7 +612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>42269</v>
       </c>
@@ -620,7 +623,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>42276</v>
       </c>
@@ -631,7 +634,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>42291</v>
       </c>
@@ -642,7 +645,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>42292</v>
       </c>
@@ -653,7 +656,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>42295</v>
       </c>
@@ -664,7 +667,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>42297</v>
       </c>
@@ -675,7 +678,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>42300</v>
       </c>
@@ -686,7 +689,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>42301</v>
       </c>
@@ -697,7 +700,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>42304</v>
       </c>
@@ -708,7 +711,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>42306</v>
       </c>
@@ -719,7 +722,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>42308</v>
       </c>
@@ -730,7 +733,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>42318</v>
       </c>
@@ -741,7 +744,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>42321</v>
       </c>
@@ -752,15 +755,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
     </row>
@@ -774,18 +773,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -796,7 +795,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>42291</v>
       </c>
@@ -807,7 +806,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>42292</v>
       </c>
@@ -818,7 +817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>42294</v>
       </c>
@@ -829,7 +828,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>42295</v>
       </c>
@@ -840,7 +839,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>42297</v>
       </c>
@@ -851,7 +850,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>42299</v>
       </c>
@@ -862,7 +861,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>42300</v>
       </c>
@@ -873,7 +872,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>42301</v>
       </c>
@@ -884,7 +883,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>42304</v>
       </c>
@@ -895,7 +894,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>42307</v>
       </c>
@@ -906,7 +905,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>42308</v>
       </c>
@@ -917,7 +916,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>42308</v>
       </c>
@@ -928,7 +927,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>42309</v>
       </c>
@@ -939,7 +938,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>42312</v>
       </c>
@@ -950,7 +949,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>42316</v>
       </c>
@@ -961,7 +960,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>42319</v>
       </c>
@@ -972,7 +971,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>42320</v>
       </c>
@@ -983,7 +982,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>42321</v>
       </c>
@@ -994,7 +993,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>42322</v>
       </c>
@@ -1005,7 +1004,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>42323</v>
       </c>
@@ -1016,71 +1015,78 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="4"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="3">
+        <v>42324</v>
+      </c>
+      <c r="B22" s="4">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="4"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="4"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="4"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
       <c r="B35" s="4"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
       <c r="B36" s="4"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
       <c r="B37" s="4"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
       <c r="B38" s="4"/>
     </row>
@@ -1098,12 +1104,12 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="52.140625" customWidth="1"/>
+    <col min="4" max="4" width="52.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1115,7 +1121,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>31</v>
       </c>
@@ -1127,7 +1133,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
@@ -1139,7 +1145,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>42015</v>
       </c>
@@ -1151,7 +1157,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>42015</v>
       </c>
@@ -1163,173 +1169,197 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="2"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B1:C1"/>
@@ -1344,30 +1374,6 @@
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1381,14 +1387,14 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1399,7 +1405,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>42299</v>
       </c>
@@ -1410,7 +1416,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>42300</v>
       </c>
@@ -1421,7 +1427,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>42302</v>
       </c>
@@ -1432,167 +1438,167 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="4"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="4"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="4"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
       <c r="B35" s="4"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
       <c r="B36" s="4"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
       <c r="B37" s="4"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="2"/>
       <c r="B38" s="4"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="2"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="2"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="2"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="2"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="2"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated TimeSheet + Added sprites to use for portal icon
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheet.xlsx
+++ b/Documentation/TimeSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="24240" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="24240" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team Meetings" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
   <si>
     <t>DATE</t>
   </si>
@@ -197,9 +197,6 @@
     <t>Significant visual overhaul + Gameplay balancing</t>
   </si>
   <si>
-    <t>Audio balancing</t>
-  </si>
-  <si>
     <t>Enemy balance + Currency distribution balance + Music track addition</t>
   </si>
   <si>
@@ -213,6 +210,21 @@
   </si>
   <si>
     <t>What was worked on</t>
+  </si>
+  <si>
+    <t>Audio balancing + Modified enemy parameters for scalability</t>
+  </si>
+  <si>
+    <t>Significant Refactoring of Map Generator to improve map layout</t>
+  </si>
+  <si>
+    <t>Balanced Map Generator + Tweaked randomization</t>
+  </si>
+  <si>
+    <t>Balanced Game for Really high levels (200+) + Major bug and stability fixes</t>
+  </si>
+  <si>
+    <t>UI Cleanup + Video Capture</t>
   </si>
 </sst>
 </file>
@@ -260,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -270,6 +282,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -583,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +622,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -807,12 +820,8 @@
         <v>0.5</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -824,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,7 +1127,7 @@
         <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1129,7 +1138,7 @@
         <v>1.5</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1140,7 +1149,7 @@
         <v>1.5</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1159,41 +1168,68 @@
         <v>42332</v>
       </c>
       <c r="B30" s="4">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="4"/>
+      <c r="A31" s="3">
+        <v>42333</v>
+      </c>
+      <c r="B31" s="4">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="4"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="4"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="4"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="4"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>42334</v>
+      </c>
+      <c r="B32" s="7">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>42335</v>
+      </c>
+      <c r="B33" s="7">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>42336</v>
+      </c>
+      <c r="B34" s="7">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="7"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="4"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="4"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="4"/>
     </row>
@@ -1220,10 +1256,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9"/>
+      <c r="C1" s="10"/>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1232,10 +1268,10 @@
       <c r="A2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="9">
         <v>3</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="9"/>
       <c r="D2" t="s">
         <v>35</v>
       </c>
@@ -1244,10 +1280,10 @@
       <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="9">
         <v>1</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="9"/>
       <c r="D3" t="s">
         <v>33</v>
       </c>
@@ -1256,10 +1292,10 @@
       <c r="A4" s="6">
         <v>42015</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="9">
         <v>3</v>
       </c>
-      <c r="C4" s="8"/>
+      <c r="C4" s="9"/>
       <c r="D4" t="s">
         <v>34</v>
       </c>
@@ -1268,181 +1304,205 @@
       <c r="A5" s="6">
         <v>42015</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="9">
         <v>1.5</v>
       </c>
-      <c r="C5" s="8"/>
+      <c r="C5" s="9"/>
       <c r="D5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B1:C1"/>
@@ -1457,30 +1517,6 @@
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Game Design Doc - FINAL
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheet.xlsx
+++ b/Documentation/TimeSheet.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericphilippona/Documents/workspace/TalosOrigins/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eprov\Documents\GitHub\TalosOrigins\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
   </bookViews>
   <sheets>
     <sheet name="Team Meetings" sheetId="4" r:id="rId1"/>
@@ -20,12 +20,10 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="93">
   <si>
     <t>DATE</t>
   </si>
@@ -224,9 +222,6 @@
     <t>Balanced Game for Really high levels (200+) + Major bug and stability fixes</t>
   </si>
   <si>
-    <t>UI Cleanup + Video Capture</t>
-  </si>
-  <si>
     <t>Add shop as canvas in main scene</t>
   </si>
   <si>
@@ -267,6 +262,54 @@
   </si>
   <si>
     <t>UI Audio</t>
+  </si>
+  <si>
+    <t>TOTAL HOURS</t>
+  </si>
+  <si>
+    <t>Meeting to discuss remaining polish</t>
+  </si>
+  <si>
+    <t>Meeting to discuss game demo</t>
+  </si>
+  <si>
+    <t>Balancing as a response to player feedback</t>
+  </si>
+  <si>
+    <t>Added multi-bullet upgrade</t>
+  </si>
+  <si>
+    <t>Work on UI</t>
+  </si>
+  <si>
+    <t>Improved UI</t>
+  </si>
+  <si>
+    <t>Added Pause Menu</t>
+  </si>
+  <si>
+    <t>Improved UI for pause menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balancing as a response to player feedback </t>
+  </si>
+  <si>
+    <t>UI Cleanup + Video Capture + Added Main Menu</t>
+  </si>
+  <si>
+    <t>30/11/15</t>
+  </si>
+  <si>
+    <t>Major UI Cleanup + Balancing of upgrade power and costs</t>
+  </si>
+  <si>
+    <t>ERIC PROVENCHER</t>
+  </si>
+  <si>
+    <t>ERIC PHILIPPONA</t>
+  </si>
+  <si>
+    <t>HU NINGGE</t>
   </si>
 </sst>
 </file>
@@ -302,7 +345,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -310,29 +353,135 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,242 +790,277 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="8">
         <v>42262</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="15">
         <v>0.5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="8">
         <v>42265</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="15">
         <v>0.25</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="8">
         <v>42267</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="15">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="8">
         <v>42269</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="15">
         <v>0.25</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="8">
         <v>42276</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="15">
         <v>0.5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="8">
         <v>42291</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="15">
         <v>1.5</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="8">
         <v>42292</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="15">
         <v>0.5</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="8">
         <v>42295</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="15">
         <v>0.25</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="8">
         <v>42297</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="15">
         <v>0.25</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="8">
         <v>42300</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="15">
         <v>1.5</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="8">
         <v>42301</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="15">
         <v>1</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="8">
         <v>42304</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="15">
         <v>0.5</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="8">
         <v>42306</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="15">
         <v>0.5</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="8">
         <v>42308</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="16">
         <v>1.5</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="8">
         <v>42318</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="15">
         <v>1</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="8">
         <v>42321</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="16">
         <v>0.5</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="8">
         <v>42325</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="15">
         <v>0.5</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="8">
         <v>42332</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="16">
         <v>0.5</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="8">
         <v>42313</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="15">
         <v>0.25</v>
       </c>
-      <c r="C21" t="s">
-        <v>65</v>
+      <c r="C21" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="8">
+        <v>42338</v>
+      </c>
+      <c r="B22" s="16">
+        <v>1</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="8">
+        <v>42339</v>
+      </c>
+      <c r="B23" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B24" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B25" s="17">
+        <f>SUM(B3:B23)</f>
+        <v>14.25</v>
       </c>
     </row>
   </sheetData>
@@ -887,407 +1071,447 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="20"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="8">
         <v>42291</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B3" s="11">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="8">
         <v>42292</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B4" s="11">
         <v>5.5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="8">
         <v>42294</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B5" s="11">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="8">
         <v>42295</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B6" s="11">
         <v>1.5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="8">
         <v>42297</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B7" s="11">
         <v>1.5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="8">
         <v>42299</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B8" s="11">
         <v>2</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="8">
         <v>42300</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B9" s="11">
         <v>3.5</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="8">
         <v>42301</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B10" s="11">
         <v>2</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="8">
         <v>42304</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B11" s="11">
         <v>1</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="8">
         <v>42307</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B12" s="11">
         <v>2</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="8">
         <v>42308</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B13" s="11">
         <v>2</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="8">
         <v>42308</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B14" s="11">
         <v>2</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="8">
         <v>42309</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B15" s="11">
         <v>1.5</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="8">
         <v>42312</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B16" s="11">
         <v>2</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="8">
         <v>42316</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B17" s="11">
         <v>3</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" s="9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="8">
         <v>42319</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B18" s="11">
         <v>2.5</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="8">
         <v>42320</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B19" s="11">
         <v>1.5</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="8">
         <v>42321</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B20" s="11">
         <v>1</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="8">
         <v>42322</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B21" s="11">
         <v>5</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" s="9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="8">
         <v>42323</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B22" s="11">
         <v>3.5</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" s="9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="8">
         <v>42324</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B23" s="11">
         <v>3</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="8">
         <v>42325</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B24" s="11">
         <v>2.5</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="8">
         <v>42326</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B25" s="11">
         <v>2</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" s="9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="8">
         <v>42327</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B26" s="11">
         <v>2.5</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="8">
         <v>42328</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B27" s="11">
         <v>2</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" s="9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="8">
         <v>42329</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B28" s="11">
         <v>1.5</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" s="9" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="8">
         <v>42330</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B29" s="11">
         <v>1.5</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" s="9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="8">
         <v>42331</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B30" s="11">
         <v>5</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="8">
         <v>42332</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B31" s="11">
         <v>5</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="8">
         <v>42333</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B32" s="11">
         <v>4</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" s="9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="8">
         <v>42334</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B33" s="11">
         <v>3</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" s="9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="8">
         <v>42335</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B34" s="11">
         <v>3</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" s="9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="8">
         <v>42336</v>
       </c>
-      <c r="B34" s="7">
+      <c r="B35" s="11">
         <v>3</v>
       </c>
-      <c r="C34" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B35" s="7"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="3"/>
-      <c r="B36" s="4"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
-      <c r="B37" s="4"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="3"/>
-      <c r="B38" s="4"/>
+      <c r="C35" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="8">
+        <v>42337</v>
+      </c>
+      <c r="B36" s="11">
+        <v>1</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="8">
+        <v>42338</v>
+      </c>
+      <c r="B37" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="8">
+        <v>42339</v>
+      </c>
+      <c r="B38" s="11">
+        <v>2</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="2"/>
+      <c r="B39" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B40" s="13">
+        <f>SUM(B3:B38)</f>
+        <v>89.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B44" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1297,565 +1521,522 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="52.1640625" customWidth="1"/>
+    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="20"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="1" t="s">
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B3" s="11">
         <v>3</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" t="s">
+      <c r="C3" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B4" s="11">
         <v>1</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" t="s">
+      <c r="C4" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="10">
         <v>42015</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B5" s="11">
         <v>4</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" t="s">
+      <c r="C5" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="10">
         <v>42015</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B6" s="11">
         <v>1.5</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" t="s">
+      <c r="C6" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="10">
         <v>42135</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B7" s="11">
         <v>3</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" t="s">
+      <c r="C7" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="10">
+        <v>42046</v>
+      </c>
+      <c r="B8" s="11">
+        <v>3</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="10">
+        <v>42288</v>
+      </c>
+      <c r="B9" s="11">
+        <v>3</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
-        <v>42046</v>
-      </c>
-      <c r="B7" s="10">
-        <v>3</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
-        <v>42288</v>
-      </c>
-      <c r="B8" s="10">
-        <v>3</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" t="s">
+      <c r="B10" s="11">
+        <v>2</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" s="10">
-        <v>2</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B10" s="10">
+      <c r="B12" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="11">
         <v>1</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" t="s">
+      <c r="C13" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" s="10">
-        <v>1.5</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B12" s="10">
+      <c r="B14" s="11">
         <v>1</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" t="s">
+      <c r="C14" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="10">
-        <v>1</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="11">
+        <v>4</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="2"/>
+      <c r="B16" s="14" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="3"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="3"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="3"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="3"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="3"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="3"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="3"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="3"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="3"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="3"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="3"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="2"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="2"/>
+      <c r="B17" s="13">
+        <f>SUM(B3:B15)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="2"/>
+      <c r="B19" s="5"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="2"/>
+      <c r="B22" s="5"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="2"/>
+      <c r="B23" s="5"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="2"/>
+      <c r="B24" s="5"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="2"/>
+      <c r="B25" s="5"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="2"/>
+      <c r="B26" s="5"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="2"/>
+      <c r="B27" s="5"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="2"/>
+      <c r="B28" s="5"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="2"/>
+      <c r="B29" s="5"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="2"/>
+      <c r="B30" s="5"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="2"/>
+      <c r="B31" s="5"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="2"/>
+      <c r="B32" s="5"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="2"/>
+      <c r="B33" s="5"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="1"/>
+      <c r="B34" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B6:C6"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection sqref="A1:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="112.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="8">
         <v>42299</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B3" s="11">
         <v>4.5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="8">
         <v>42300</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B4" s="11">
         <v>2.5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="8">
         <v>42302</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B5" s="11">
         <v>4.5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" s="9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
-      <c r="B22" s="4"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
-      <c r="B25" s="4"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="3"/>
-      <c r="B27" s="4"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="3"/>
-      <c r="B28" s="4"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="3"/>
-      <c r="B30" s="4"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="3"/>
-      <c r="B31" s="4"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="3"/>
-      <c r="B32" s="4"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="3"/>
-      <c r="B33" s="4"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="3"/>
-      <c r="B34" s="4"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="3"/>
-      <c r="B35" s="4"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="3"/>
-      <c r="B36" s="4"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
-      <c r="B37" s="4"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="8">
+        <v>42330</v>
+      </c>
+      <c r="B6" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="8">
+        <v>42331</v>
+      </c>
+      <c r="B7" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="8">
+        <v>42337</v>
+      </c>
+      <c r="B8" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="8">
+        <v>42338</v>
+      </c>
+      <c r="B9" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="2"/>
+      <c r="B10" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="2"/>
+      <c r="B11" s="13">
+        <f>SUM(B3:B9)</f>
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="2"/>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="2"/>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="2"/>
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="2"/>
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="2"/>
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="2"/>
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="2"/>
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="2"/>
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="2"/>
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="2"/>
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="2"/>
+      <c r="B29" s="3"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="2"/>
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="2"/>
+      <c r="B32" s="3"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="2"/>
+      <c r="B33" s="3"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="2"/>
+      <c r="B34" s="3"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="2"/>
+      <c r="B35" s="3"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="2"/>
+      <c r="B36" s="3"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="2"/>
+      <c r="B37" s="3"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="2"/>
-      <c r="B38" s="4"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="2"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="2"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="2"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="2"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="2"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="2"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="2"/>
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="1"/>
+      <c r="B39" s="3"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" s="1"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" s="1"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" s="1"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" s="1"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" s="1"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" s="1"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" s="1"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Game Design Doc
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheet.xlsx
+++ b/Documentation/TimeSheet.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eprov\Documents\GitHub\TalosOrigins\Documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team Meetings" sheetId="4" r:id="rId1"/>
@@ -15,7 +20,7 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="96">
   <si>
     <t>DATE</t>
   </si>
@@ -310,12 +315,15 @@
   </si>
   <si>
     <t>write document</t>
+  </si>
+  <si>
+    <t>Rebalanced Game Entropy + Polished UI + Fixed New Game Bugs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yy/mm/dd;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -345,7 +353,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -449,11 +457,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -497,9 +518,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -797,7 +822,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1088,8 +1113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1514,15 +1539,25 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="12" t="s">
+      <c r="A39" s="25">
+        <v>42342</v>
+      </c>
+      <c r="B39" s="26">
+        <v>4.5</v>
+      </c>
+      <c r="C39" s="24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="12" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="13">
-        <f>SUM(B3:B38)</f>
-        <v>89.5</v>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="13">
+        <f>SUM(B3:B39)</f>
+        <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1798,7 +1833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>

</xml_diff>